<commit_message>
added download input template
</commit_message>
<xml_diff>
--- a/output (1).xlsx
+++ b/output (1).xlsx
@@ -742,31 +742,31 @@
         <v>70</v>
       </c>
       <c r="Z2" t="n">
-        <v>9012.15</v>
+        <v>9047.290000000001</v>
       </c>
       <c r="AA2" t="n">
-        <v>17955.71</v>
+        <v>17936.14</v>
       </c>
       <c r="AB2" t="n">
-        <v>30230.88</v>
+        <v>29953.73</v>
       </c>
       <c r="AC2" t="n">
-        <v>1577.36</v>
+        <v>1574.46</v>
       </c>
       <c r="AD2" t="n">
-        <v>3489.54</v>
+        <v>3479.21</v>
       </c>
       <c r="AE2" t="n">
-        <v>6416.44</v>
+        <v>6451.09</v>
       </c>
       <c r="AF2" t="n">
-        <v>270.52</v>
+        <v>270.02</v>
       </c>
       <c r="AG2" t="n">
-        <v>598.46</v>
+        <v>596.6799999999999</v>
       </c>
       <c r="AH2" t="n">
-        <v>1100.42</v>
+        <v>1106.36</v>
       </c>
       <c r="AI2" t="n">
         <v>17.15</v>
@@ -881,34 +881,34 @@
       </c>
       <c r="AK3" t="inlineStr"/>
       <c r="AL3" t="n">
-        <v>856516.49</v>
+        <v>851602.03</v>
       </c>
       <c r="AM3" t="n">
-        <v>1336437.45</v>
+        <v>1338653.04</v>
       </c>
       <c r="AN3" t="n">
-        <v>2053306.11</v>
+        <v>2046895.33</v>
       </c>
       <c r="AO3" t="n">
-        <v>146414.62</v>
+        <v>145949.29</v>
       </c>
       <c r="AP3" t="n">
-        <v>262076.41</v>
+        <v>262358.11</v>
       </c>
       <c r="AQ3" t="n">
-        <v>446136.01</v>
+        <v>446075.91</v>
       </c>
       <c r="AR3" t="n">
-        <v>24597.66</v>
+        <v>24519.48</v>
       </c>
       <c r="AS3" t="n">
-        <v>44028.84</v>
+        <v>44076.16</v>
       </c>
       <c r="AT3" t="n">
-        <v>74950.85000000001</v>
+        <v>74940.75</v>
       </c>
       <c r="AU3" t="n">
-        <v>10480.4</v>
+        <v>10495.7</v>
       </c>
     </row>
     <row r="4">
@@ -988,31 +988,31 @@
         <v>80</v>
       </c>
       <c r="Z4" t="n">
-        <v>11416.46</v>
+        <v>11632.29</v>
       </c>
       <c r="AA4" t="n">
-        <v>16773.41</v>
+        <v>16692.12</v>
       </c>
       <c r="AB4" t="n">
-        <v>23190.53</v>
+        <v>23168.78</v>
       </c>
       <c r="AC4" t="n">
-        <v>1253.5</v>
+        <v>1280.04</v>
       </c>
       <c r="AD4" t="n">
-        <v>2447.46</v>
+        <v>2449.43</v>
       </c>
       <c r="AE4" t="n">
-        <v>4074</v>
+        <v>4026.97</v>
       </c>
       <c r="AF4" t="n">
-        <v>442.23</v>
+        <v>451.6</v>
       </c>
       <c r="AG4" t="n">
-        <v>863.46</v>
+        <v>864.16</v>
       </c>
       <c r="AH4" t="n">
-        <v>1437.31</v>
+        <v>1420.72</v>
       </c>
       <c r="AI4" t="n">
         <v>35.28</v>

</xml_diff>